<commit_message>
- meer conversie info
</commit_message>
<xml_diff>
--- a/source/sap2exact/sap2exact/conversie.xlsx
+++ b/source/sap2exact/sap2exact/conversie.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>EindArtikel</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>geel is nog invullen</t>
+  </si>
+  <si>
+    <t>EindArtikel fallback (wanneer niet met een cijfer begint)</t>
   </si>
 </sst>
 </file>
@@ -517,15 +520,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="12.140625" style="3"/>
+    <col min="1" max="3" width="12.140625" style="3"/>
+    <col min="4" max="4" width="28.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -570,11 +576,11 @@
       <c r="C2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="3">
-        <v>69</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>69</v>
       </c>
       <c r="F2" s="3">
         <v>6600</v>
@@ -602,11 +608,11 @@
       <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3">
-        <v>69</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>69</v>
       </c>
       <c r="F3" s="3">
         <v>6610</v>
@@ -634,11 +640,11 @@
       <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="3">
-        <v>69</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="E4" s="3">
+        <v>69</v>
       </c>
       <c r="F4" s="3">
         <v>6620</v>
@@ -666,11 +672,11 @@
       <c r="C5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="3">
-        <v>69</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="E5" s="3">
+        <v>69</v>
       </c>
       <c r="F5" s="3">
         <v>6630</v>
@@ -698,11 +704,11 @@
       <c r="C6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="3">
-        <v>69</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="E6" s="3">
+        <v>69</v>
       </c>
       <c r="F6" s="3">
         <v>6640</v>
@@ -730,11 +736,11 @@
       <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3">
-        <v>69</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>69</v>
       </c>
       <c r="F7" s="3">
         <v>6650</v>
@@ -762,11 +768,11 @@
       <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="3">
-        <v>69</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>69</v>
       </c>
       <c r="F8" s="3">
         <v>6660</v>
@@ -794,11 +800,11 @@
       <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3">
-        <v>69</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="E9" s="3">
+        <v>69</v>
       </c>
       <c r="F9" s="3">
         <v>6670</v>
@@ -826,11 +832,11 @@
       <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="3">
-        <v>69</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="E10" s="3">
+        <v>69</v>
       </c>
       <c r="F10" s="3">
         <v>6680</v>
@@ -858,11 +864,11 @@
       <c r="C11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="3">
-        <v>69</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="E11" s="3">
+        <v>69</v>
       </c>
       <c r="F11" s="3">
         <v>6690</v>
@@ -882,45 +888,45 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4">
-        <v>69</v>
-      </c>
-      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="E12" s="4">
+        <v>69</v>
+      </c>
       <c r="F12" s="4">
-        <v>6630</v>
+        <v>6690</v>
       </c>
       <c r="G12" s="4">
-        <v>86200</v>
+        <v>86690</v>
       </c>
       <c r="H12" s="4">
-        <v>30620</v>
+        <v>30669</v>
       </c>
       <c r="I12" s="4">
-        <v>76200</v>
+        <v>76690</v>
       </c>
       <c r="J12" s="4">
-        <v>81020</v>
+        <v>81069</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="4">
-        <v>69</v>
-      </c>
-      <c r="E13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="E13" s="4">
+        <v>69</v>
       </c>
       <c r="F13" s="4">
         <v>6630</v>
@@ -940,16 +946,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="4">
-        <v>69</v>
-      </c>
-      <c r="E14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="E14" s="4">
+        <v>69</v>
       </c>
       <c r="F14" s="4">
         <v>6630</v>
@@ -963,22 +969,22 @@
       <c r="I14" s="4">
         <v>76200</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>28</v>
+      <c r="J14" s="4">
+        <v>81020</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="4">
-        <v>69</v>
-      </c>
-      <c r="E15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="E15" s="4">
+        <v>69</v>
       </c>
       <c r="F15" s="4">
         <v>6630</v>
@@ -996,8 +1002,37 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="4">
+        <v>69</v>
+      </c>
+      <c r="F16" s="4">
+        <v>6630</v>
+      </c>
+      <c r="G16" s="4">
+        <v>86200</v>
+      </c>
+      <c r="H16" s="4">
+        <v>30620</v>
+      </c>
+      <c r="I16" s="4">
+        <v>76200</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>